<commit_message>
Changed the structure of tgBot
</commit_message>
<xml_diff>
--- a/users_data/794329884_order.xlsx
+++ b/users_data/794329884_order.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Astrocatling\WBbot\users_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Astrocatling\WBbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAD5E67-9E09-4347-BF78-AD036548E5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F15A0A3-A353-43A6-AF71-B938BF0E0D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="3000" windowWidth="28100" windowHeight="15910" xr2:uid="{3D39B954-54E1-433D-BDD4-09D5FB40C627}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Серьги для девочек</t>
   </si>
@@ -56,22 +56,13 @@
   </si>
   <si>
     <t>г. Москва, м Семёновская, Измайловское шоссе, д. 6</t>
-  </si>
-  <si>
-    <t>г. Москва, м Семёновская, Измайловское шоссе, д. 5</t>
-  </si>
-  <si>
-    <t>г. Москва, м Семёновская, Измайловское шоссе, д. 4</t>
-  </si>
-  <si>
-    <t>г. Москва, м Семёновская, Измайловское шоссе, д. 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +75,13 @@
       <sz val="10"/>
       <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="7"/>
@@ -113,12 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -433,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC5D944-6DD4-458D-AE01-0CEC5CCC11F0}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -469,17 +468,17 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>44398622</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>123</v>
@@ -489,21 +488,11 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2"/>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2"/>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>